<commit_message>
added pv fk's to schema and updated demo data
</commit_message>
<xml_diff>
--- a/protected/data/excel/person.xlsx
+++ b/protected/data/excel/person.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="216">
   <si>
     <t>First Name</t>
   </si>
@@ -664,9 +664,6 @@
     <t>Profile1</t>
   </si>
   <si>
-    <t>Nick</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -701,6 +698,12 @@
   </si>
   <si>
     <t>profile</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>nick</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1820,7 +1823,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="72" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>198</v>
@@ -1860,7 +1863,7 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>0</v>
@@ -1884,10 +1887,10 @@
         <v>201</v>
       </c>
       <c r="I2" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="J2" s="53" t="s">
         <v>212</v>
-      </c>
-      <c r="J2" s="53" t="s">
-        <v>213</v>
       </c>
       <c r="K2" s="33" t="s">
         <v>13</v>
@@ -3858,7 +3861,7 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>195</v>
@@ -3902,31 +3905,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="47" t="s">
-        <v>204</v>
-      </c>
       <c r="C1" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="47" t="s">
-        <v>209</v>
-      </c>
       <c r="I1" s="47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3959,8 +3962,8 @@
         <v>Barcoe</v>
       </c>
       <c r="H2" s="64" t="str">
-        <f>CONCATENATE(LEFT(F2,1),LEFT(G2,1))</f>
-        <v>JB</v>
+        <f>CONCATENATE(LEFT(G2,1),LEFT(F2,1))</f>
+        <v>BJ</v>
       </c>
       <c r="I2" s="65">
         <f>Master!I3</f>
@@ -3997,8 +4000,8 @@
         <v>Barton</v>
       </c>
       <c r="H3" s="64" t="str">
-        <f t="shared" ref="H3:I23" si="0">CONCATENATE(LEFT(F3,1),LEFT(G3,1))</f>
-        <v>SB</v>
+        <f t="shared" ref="H3:H23" si="0">CONCATENATE(LEFT(G3,1),LEFT(F3,1))</f>
+        <v>BS</v>
       </c>
       <c r="I3" s="64">
         <f>Master!I4</f>
@@ -4036,7 +4039,7 @@
       </c>
       <c r="H4" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>AB</v>
+        <v>BA</v>
       </c>
       <c r="I4" s="64">
         <f>Master!I5</f>
@@ -4074,7 +4077,7 @@
       </c>
       <c r="H5" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>MF</v>
+        <v>FM</v>
       </c>
       <c r="I5" s="64">
         <f>Master!I6</f>
@@ -4112,7 +4115,7 @@
       </c>
       <c r="H6" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>JG</v>
+        <v>GJ</v>
       </c>
       <c r="I6" s="64">
         <f>Master!I7</f>
@@ -4150,7 +4153,7 @@
       </c>
       <c r="H7" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>BH</v>
+        <v>HB</v>
       </c>
       <c r="I7" s="64">
         <f>Master!I8</f>
@@ -4188,7 +4191,7 @@
       </c>
       <c r="H8" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>RH</v>
+        <v>HR</v>
       </c>
       <c r="I8" s="64">
         <f>Master!I9</f>
@@ -4226,7 +4229,7 @@
       </c>
       <c r="H9" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>WJ</v>
+        <v>JW</v>
       </c>
       <c r="I9" s="64">
         <f>Master!I10</f>
@@ -4264,7 +4267,7 @@
       </c>
       <c r="H10" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>PJ</v>
+        <v>JP</v>
       </c>
       <c r="I10" s="64">
         <f>Master!I11</f>
@@ -4302,7 +4305,7 @@
       </c>
       <c r="H11" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>HJ</v>
+        <v>JH</v>
       </c>
       <c r="I11" s="64">
         <f>Master!I12</f>
@@ -4340,7 +4343,7 @@
       </c>
       <c r="H12" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>MJ</v>
+        <v>JM</v>
       </c>
       <c r="I12" s="64">
         <f>Master!I13</f>
@@ -4378,7 +4381,7 @@
       </c>
       <c r="H13" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>SJ</v>
+        <v>JS</v>
       </c>
       <c r="I13" s="64">
         <f>Master!I14</f>
@@ -4416,7 +4419,7 @@
       </c>
       <c r="H14" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>BM</v>
+        <v>MB</v>
       </c>
       <c r="I14" s="64">
         <f>Master!I15</f>
@@ -4454,7 +4457,7 @@
       </c>
       <c r="H15" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>NM</v>
+        <v>MN</v>
       </c>
       <c r="I15" s="64">
         <f>Master!I16</f>
@@ -4492,7 +4495,7 @@
       </c>
       <c r="H16" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>BM</v>
+        <v>MB</v>
       </c>
       <c r="I16" s="64">
         <f>Master!I17</f>
@@ -4530,7 +4533,7 @@
       </c>
       <c r="H17" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>DM</v>
+        <v>MD</v>
       </c>
       <c r="I17" s="64">
         <f>Master!I18</f>
@@ -4606,7 +4609,7 @@
       </c>
       <c r="H19" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>SR</v>
+        <v>RS</v>
       </c>
       <c r="I19" s="64">
         <f>Master!I20</f>
@@ -4644,7 +4647,7 @@
       </c>
       <c r="H20" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>MS</v>
+        <v>SM</v>
       </c>
       <c r="I20" s="64">
         <f>Master!I21</f>
@@ -4682,7 +4685,7 @@
       </c>
       <c r="H21" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>ST</v>
+        <v>TS</v>
       </c>
       <c r="I21" s="64">
         <f>Master!I22</f>
@@ -4720,7 +4723,7 @@
       </c>
       <c r="H22" s="64" t="str">
         <f t="shared" si="0"/>
-        <v>DW</v>
+        <v>WD</v>
       </c>
       <c r="I22" s="64">
         <f>Master!I23</f>
@@ -4758,7 +4761,7 @@
       </c>
       <c r="H23" s="67" t="str">
         <f t="shared" si="0"/>
-        <v>CW</v>
+        <v>WC</v>
       </c>
       <c r="I23" s="67">
         <f>Master!I24</f>

</xml_diff>